<commit_message>
Função Naive Bayes e verificação ainda não funcionais
</commit_message>
<xml_diff>
--- a/McDonalds(1).xlsx
+++ b/McDonalds(1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Desktop\Leca\Insper\Matérias\2o Semestre\Ciência de Dados\Ciencia_dos_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="435">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1354,13 +1354,16 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Relevância</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1380,6 +1383,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1426,7 +1437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1434,6 +1445,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1774,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="B320" sqref="B320"/>
+    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,12 +1799,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>432</v>
       </c>
     </row>
@@ -4316,6 +4331,7 @@
     <hyperlink ref="A54" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4323,18 +4339,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="130.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>264</v>
+      </c>
+      <c r="B1" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -6035,11 +6055,11 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
+      <c r="A201" s="3" t="s">
         <v>431</v>
       </c>
       <c r="B201" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>